<commit_message>
19 20 21  （12:10）
</commit_message>
<xml_diff>
--- a/Excel/StartSceneConfig@s.xlsx
+++ b/Excel/StartSceneConfig@s.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CLKProjects\UnityProjects\Study\ETStudy\ETSLGGame\ET-EUI\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D123D4FA-DBDA-4958-80F7-466015830169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC98AAED-C321-4CAE-B4AC-0516697B2B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="765" windowWidth="22215" windowHeight="14835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
   <si>
     <t>Id</t>
   </si>
@@ -93,6 +93,10 @@
   </si>
   <si>
     <t>Account</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoginCenter</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -483,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:H12"/>
+  <dimension ref="C3:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -693,10 +697,28 @@
         <v>10005</v>
       </c>
     </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C13" s="3">
+        <v>8</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>